<commit_message>
fix: the word day hours is 8 hours
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/new/PycharmProjects/calc_sla/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FBF2A04-6BE6-4D4D-9DC0-A985B2F98A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9524B0-D34F-054F-8021-E92CE7783308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="500" windowWidth="37320" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
   <si>
     <t>创建日期</t>
   </si>
@@ -47,6 +47,69 @@
   </si>
   <si>
     <t>最终结果（h）1</t>
+  </si>
+  <si>
+    <t>2022/05/16 08:00:00</t>
+  </si>
+  <si>
+    <t>2022/05/16 17:00:00</t>
+  </si>
+  <si>
+    <t>2022/05/16 08:30:00</t>
+  </si>
+  <si>
+    <t>2022/05/16 09:00:00</t>
+  </si>
+  <si>
+    <t>2022/05/16 18:00:00</t>
+  </si>
+  <si>
+    <t>2022/05/16 19:00:00</t>
+  </si>
+  <si>
+    <t>2022/05/16 13:00:00</t>
+  </si>
+  <si>
+    <t>2022/05/05 08:00:00</t>
+  </si>
+  <si>
+    <t>2022/05/06 17:00:00</t>
+  </si>
+  <si>
+    <t>2022/05/05 08:30:00</t>
+  </si>
+  <si>
+    <t>2022/05/05 09:00:00</t>
+  </si>
+  <si>
+    <t>2022/05/06 18:00:00</t>
+  </si>
+  <si>
+    <t>2022/05/06 19:00:00</t>
+  </si>
+  <si>
+    <t>2022/05/05 13:00:00</t>
+  </si>
+  <si>
+    <t>2022/06/02 08:00:00</t>
+  </si>
+  <si>
+    <t>2022/06/06 17:00:00</t>
+  </si>
+  <si>
+    <t>2022/06/02 08:30:00</t>
+  </si>
+  <si>
+    <t>2022/06/02 09:00:00</t>
+  </si>
+  <si>
+    <t>2022/06/06 18:00:00</t>
+  </si>
+  <si>
+    <t>2022/06/06 19:00:00</t>
+  </si>
+  <si>
+    <t>2022/06/03 08:00:00</t>
   </si>
 </sst>
 </file>
@@ -54,22 +117,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="182" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="180" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Microsoft YaHei Light"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -79,21 +135,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -101,40 +151,36 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="22" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -405,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B9"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -434,79 +480,275 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18">
-      <c r="A2" s="1">
-        <v>44697.352835648097</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44697.712754629603</v>
-      </c>
-      <c r="C2" s="4">
-        <f>B2-A2</f>
-        <v>0.35991898150678026</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18">
-      <c r="A3" s="1">
-        <v>44697.7050578704</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44698.448738425897</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18">
-      <c r="A4" s="1">
-        <v>44701.7046527778</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44704.718773148103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18">
-      <c r="A5" s="1">
-        <v>44684.396203703698</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44686.587280092601</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18">
-      <c r="A6" s="2">
-        <v>44796.503842592603</v>
-      </c>
-      <c r="B6" s="2">
-        <v>44796.878842592603</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18">
-      <c r="A7" s="2">
-        <v>44796.292037036997</v>
-      </c>
-      <c r="B7" s="2">
-        <v>44797.878842592603</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="18">
-      <c r="A8" s="2">
-        <v>44645.377604166701</v>
-      </c>
-      <c r="B8" s="2">
-        <v>44650.677418981497</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="18">
-      <c r="A9" s="2">
-        <v>44646.458402777796</v>
-      </c>
-      <c r="B9" s="2">
-        <v>44649.387326388904</v>
-      </c>
-    </row>
-    <row r="21" spans="8:8">
-      <c r="H21" s="3"/>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="2">
+        <v>44697.791666666664</v>
+      </c>
+      <c r="B32" s="2">
+        <v>44697.833333333336</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2">
+        <v>44697.520833333336</v>
+      </c>
+      <c r="B33" s="2">
+        <v>44697.541666666664</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A2:B31">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$A2=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32:B33">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A32=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>